<commit_message>
update development record file
</commit_message>
<xml_diff>
--- a/pc/src/main/doc/sql/DB设计.xlsx
+++ b/pc/src/main/doc/sql/DB设计.xlsx
@@ -4,21 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="用户表设计(USER)" sheetId="1" r:id="rId1"/>
     <sheet name="表达式(EXPRESSION)" sheetId="2" r:id="rId2"/>
-    <sheet name="年级表(GRADE)" sheetId="3" r:id="rId3"/>
-    <sheet name="学生_年级表（STU_GRADE)" sheetId="4" r:id="rId4"/>
-    <sheet name="做题记录表(record)" sheetId="5" r:id="rId5"/>
+    <sheet name="做题记录表(record)" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>字段名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -172,11 +170,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>班级名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(30)</t>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不为空，自增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表达式序列号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">不为空 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户序列号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">不为空 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户给出的答案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -184,11 +230,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>u_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户序列号</t>
+    <t>r_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户做题时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(25)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e_tip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>做题提示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长度&lt;=100,可以为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户是第几次做题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">INT </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_rank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>题目难度等级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -196,83 +286,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>外键</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不为空，自增</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主键</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表达式序列号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">不为空 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>u_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户序列号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">不为空 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户给出的答案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(10)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不为空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户做题时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>g_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>年级序列号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>g_id</t>
+    <t>分为五个等级 ， 分别是 1，2，3，4，5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -630,7 +648,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -738,7 +756,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
@@ -827,6 +845,20 @@
         <v>35</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -836,14 +868,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -866,233 +900,112 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
         <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>60</v>
       </c>
-      <c r="D6" t="s">
-        <v>57</v>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>